<commit_message>
Published state of ETDataset on October 7 2020
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_heat_network_storage.xlsx
+++ b/nodes_source_analyses/energy/energy_heat_network_storage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/nodes_source_analyses/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8953592C-5F34-CB4C-B9FC-180F4D72097A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537B535E-3518-C04F-9F4F-A0088BA958A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25580" yWindow="480" windowWidth="25600" windowHeight="28340" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19340" yWindow="460" windowWidth="30800" windowHeight="28340" tabRatio="762" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>Source</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Subject year</t>
   </si>
   <si>
     <t>ETM Library URL</t>
@@ -208,27 +205,15 @@
     <t>Kalavasta</t>
   </si>
   <si>
-    <t>Berenschot 2017</t>
-  </si>
-  <si>
     <t>energy_heat_network_storage.central_producer.ad</t>
   </si>
   <si>
     <t>Marlieke Verweij</t>
   </si>
   <si>
-    <t>Hogetemerpatuur Aquifer Thermal Storage (HT-ATES)</t>
-  </si>
-  <si>
-    <t>Daarom worden gemiddelde waarden aangenomen</t>
-  </si>
-  <si>
     <t>cost_per_mwh</t>
   </si>
   <si>
-    <t>Vermogen en opslag volume van deze opslag volgt uit berekening wat nodig is</t>
-  </si>
-  <si>
     <t>See https://github.com/quintel/documentation/blob/master/general/cost_calculations.md#weighted-average-cost-of-capital</t>
   </si>
   <si>
@@ -241,27 +226,6 @@
     <t>Ecovat</t>
   </si>
   <si>
-    <t>Kosten bron: DAREL</t>
-  </si>
-  <si>
-    <t>Verliezen bron: Ecovat</t>
-  </si>
-  <si>
-    <t>Ecovat heeft jaarlijks gemiddeld 15% verliezen (interview Ecovat)</t>
-  </si>
-  <si>
-    <t>In het ETM kan je verliezen per uur instellen, dus deze jaarlijkse verliezen moeten we terugrekenen per uur</t>
-  </si>
-  <si>
-    <t>verliezen per jaar</t>
-  </si>
-  <si>
-    <t>uur per jaar</t>
-  </si>
-  <si>
-    <t>verliezen per uur</t>
-  </si>
-  <si>
     <t>volume is afhankelijk van mismatch tussen supply en demand</t>
   </si>
   <si>
@@ -278,6 +242,72 @@
   </si>
   <si>
     <t>MW</t>
+  </si>
+  <si>
+    <t>https://www.ecovat.eu/nieuws/ecovat-vergelijkt-zichzelf-met-alternatieve-opslagsystemen/</t>
+  </si>
+  <si>
+    <t>July 2020</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Economic and thermal performance of Ecovat and comparable thermal energy storage technolgoies</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>cost per GJ</t>
+  </si>
+  <si>
+    <t>euro/GJ</t>
+  </si>
+  <si>
+    <t>Darel</t>
+  </si>
+  <si>
+    <t>ATES</t>
+  </si>
+  <si>
+    <t>https://refman.energytransitionmodel.com/publications/2125</t>
+  </si>
+  <si>
+    <t>excluding heat loss compensation costs. ETM takes these into account separately</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (if heat is lost in storage, ETM will automatically increase supply to make sure supply and demand match)</t>
+  </si>
+  <si>
+    <t>Losses:</t>
+  </si>
+  <si>
+    <t>Costs source: Ecovat</t>
+  </si>
+  <si>
+    <t>loss per year</t>
+  </si>
+  <si>
+    <t>hours per year</t>
+  </si>
+  <si>
+    <t>losses per hour</t>
+  </si>
+  <si>
+    <t>ETM uses losses per hour</t>
+  </si>
+  <si>
+    <t>High Temperature Aquifer Thermal Storage (HT-ATES)</t>
+  </si>
+  <si>
+    <t>Required capacity and volume depend on scenario in ETM and are calculated automatically by the model</t>
+  </si>
+  <si>
+    <t>Based on Ecovat interview, losses for ATES</t>
+  </si>
+  <si>
+    <t>Ecovat: "Typical efficiency for ATES: 70 %, BTES: 50 %, PTES: 75 %, TTES: 70 %, Ecovat: 90 %"</t>
   </si>
 </sst>
 </file>
@@ -288,14 +318,28 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000000000000"/>
-    <numFmt numFmtId="172" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -460,6 +504,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Montserrat Light"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Lettertype hoofdtekst"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -742,448 +797,455 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="250">
+  <cellStyleXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="177" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="177" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="18" xfId="250" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="250">
+  <cellStyles count="251">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1434,6 +1496,7 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="250" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1452,16 +1515,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>23090</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>161637</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>427178</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>276513</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>33037</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>92362</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>79206</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1484,8 +1547,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7585363" y="2667001"/>
-          <a:ext cx="10759787" cy="6937218"/>
+          <a:off x="8151087" y="7620001"/>
+          <a:ext cx="6938820" cy="4524205"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1497,15 +1560,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>819725</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>40145</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>686376</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>132508</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1528,8 +1591,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7508875" y="984250"/>
-          <a:ext cx="10058400" cy="2167395"/>
+          <a:off x="8936180" y="12028542"/>
+          <a:ext cx="8491105" cy="1831511"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1541,15 +1604,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>669636</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>30357</xdr:rowOff>
+      <xdr:colOff>738909</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>11487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>6456</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>687638</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>5774</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1572,8 +1635,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7677727" y="9601539"/>
-          <a:ext cx="11783975" cy="6567870"/>
+          <a:off x="8855364" y="13739032"/>
+          <a:ext cx="8573183" cy="4774106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>607729</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>46182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>496455</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B28C9E2-EC78-E444-9C93-3F88C41A46F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9139820" y="265546"/>
+          <a:ext cx="6354180" cy="4941454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2060,7 +2167,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2069,7 +2176,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2208,8 +2315,8 @@
   </sheetPr>
   <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2235,39 +2342,39 @@
       <c r="H1" s="31"/>
     </row>
     <row r="2" spans="2:11">
-      <c r="B2" s="109" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="111"/>
+      <c r="B2" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="124"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="112"/>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="127"/>
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="112"/>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="114"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="115"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="117"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="130"/>
       <c r="F5" s="31"/>
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
@@ -2333,7 +2440,7 @@
     </row>
     <row r="11" spans="2:11" ht="17" thickBot="1">
       <c r="B11" s="35"/>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="94" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="18" t="s">
@@ -2345,14 +2452,14 @@
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
-      <c r="I11" s="94"/>
+      <c r="I11" s="93"/>
       <c r="J11" s="65"/>
       <c r="K11" s="31"/>
     </row>
     <row r="12" spans="2:11" ht="17" thickBot="1">
       <c r="B12" s="35"/>
-      <c r="C12" s="95" t="s">
-        <v>69</v>
+      <c r="C12" s="94" t="s">
+        <v>57</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>1</v>
@@ -2364,84 +2471,84 @@
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
-      <c r="I12" s="94"/>
+      <c r="I12" s="93"/>
       <c r="J12" s="65"/>
       <c r="K12" s="31"/>
     </row>
     <row r="13" spans="2:11" ht="17" thickBot="1">
       <c r="B13" s="35"/>
-      <c r="C13" s="95" t="s">
-        <v>45</v>
+      <c r="C13" s="94" t="s">
+        <v>44</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="36">
         <f>'Research data'!G7</f>
         <v>0</v>
       </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="95"/>
+      <c r="G13" s="94"/>
       <c r="H13" s="34"/>
-      <c r="I13" s="94"/>
+      <c r="I13" s="93"/>
       <c r="J13" s="65"/>
     </row>
     <row r="14" spans="2:11" ht="17" thickBot="1">
       <c r="B14" s="35"/>
-      <c r="C14" s="104" t="s">
-        <v>46</v>
+      <c r="C14" s="103" t="s">
+        <v>45</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="36">
         <f>'Research data'!G8</f>
-        <v>20</v>
+        <v>43.2</v>
       </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="95"/>
+      <c r="G14" s="94"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="125" t="s">
-        <v>70</v>
+      <c r="I14" s="114" t="s">
+        <v>58</v>
       </c>
       <c r="J14" s="65"/>
     </row>
     <row r="15" spans="2:11" ht="17" thickBot="1">
       <c r="B15" s="35"/>
-      <c r="C15" s="124" t="s">
-        <v>57</v>
+      <c r="C15" s="113" t="s">
+        <v>52</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="36">
+        <v>53</v>
+      </c>
+      <c r="E15" s="133">
         <f>'Research data'!G9</f>
-        <v>1.8552217117551173E-5</v>
+        <v>4.0715488903164676E-5</v>
       </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="95"/>
+      <c r="G15" s="94"/>
       <c r="H15" s="34"/>
-      <c r="I15" s="125" t="s">
-        <v>59</v>
+      <c r="I15" s="114" t="s">
+        <v>54</v>
       </c>
       <c r="J15" s="65"/>
     </row>
     <row r="16" spans="2:11" ht="17" thickBot="1">
       <c r="B16" s="35"/>
-      <c r="C16" s="124" t="s">
-        <v>68</v>
+      <c r="C16" s="113" t="s">
+        <v>56</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="126">
+        <v>60</v>
+      </c>
+      <c r="E16" s="115">
         <v>1000000000000000</v>
       </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="95"/>
+      <c r="G16" s="94"/>
       <c r="H16" s="34"/>
-      <c r="I16" s="125" t="s">
-        <v>71</v>
+      <c r="I16" s="114" t="s">
+        <v>59</v>
       </c>
       <c r="J16" s="65"/>
     </row>
@@ -2477,7 +2584,7 @@
       <c r="D19" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="127">
+      <c r="E19" s="116">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F19" s="34"/>
@@ -2485,8 +2592,8 @@
         <v>13</v>
       </c>
       <c r="H19" s="34"/>
-      <c r="I19" s="108" t="s">
-        <v>56</v>
+      <c r="I19" s="106" t="s">
+        <v>51</v>
       </c>
       <c r="J19" s="65"/>
     </row>
@@ -2529,7 +2636,7 @@
   <dimension ref="B1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2578,13 +2685,13 @@
       </c>
       <c r="H3" s="44"/>
       <c r="I3" s="44" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="L3" s="44" t="s">
         <v>40</v>
@@ -2620,10 +2727,10 @@
     </row>
     <row r="6" spans="2:12" ht="17" thickBot="1">
       <c r="B6" s="76"/>
-      <c r="C6" s="118" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="96" t="s">
+      <c r="C6" s="107" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="95" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="80">
@@ -2636,62 +2743,66 @@
     </row>
     <row r="7" spans="2:12" ht="16" customHeight="1" thickBot="1">
       <c r="B7" s="76"/>
-      <c r="C7" s="123" t="s">
-        <v>45</v>
+      <c r="C7" s="112" t="s">
+        <v>44</v>
       </c>
       <c r="D7" s="73"/>
       <c r="E7" s="73"/>
-      <c r="F7" s="100" t="s">
-        <v>47</v>
+      <c r="F7" s="99" t="s">
+        <v>46</v>
       </c>
       <c r="G7" s="80">
         <v>0</v>
       </c>
-      <c r="L7" s="122" t="s">
-        <v>67</v>
+      <c r="L7" s="111" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="16" customHeight="1" thickBot="1">
       <c r="B8" s="76"/>
-      <c r="C8" s="123" t="s">
-        <v>46</v>
+      <c r="C8" s="112" t="s">
+        <v>45</v>
       </c>
       <c r="D8" s="73"/>
       <c r="E8" s="73"/>
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="101">
-        <f>I8</f>
+      <c r="G8" s="100">
+        <f>K8</f>
+        <v>43.2</v>
+      </c>
+      <c r="I8" s="104">
+        <f>Notes!E45</f>
         <v>20</v>
       </c>
-      <c r="I8" s="105">
-        <f>Notes!E11</f>
-        <v>20</v>
-      </c>
       <c r="J8" s="71"/>
+      <c r="K8" s="104">
+        <f>Notes!E8</f>
+        <v>43.2</v>
+      </c>
       <c r="L8" s="82"/>
     </row>
     <row r="9" spans="2:12" ht="18" customHeight="1" thickBot="1">
       <c r="B9" s="76"/>
       <c r="C9" s="72" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" s="83"/>
       <c r="E9" s="83"/>
-      <c r="F9" s="119" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="101">
+      <c r="F9" s="108" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="100">
         <f>K9</f>
-        <v>1.8552217117551173E-5</v>
+        <v>4.0715488903164676E-5</v>
       </c>
       <c r="H9" s="84"/>
       <c r="I9" s="84"/>
       <c r="J9" s="84"/>
-      <c r="K9" s="105">
+      <c r="K9" s="104">
         <f>Notes!E28</f>
-        <v>1.8552217117551173E-5</v>
+        <v>4.0715488903164676E-5</v>
       </c>
       <c r="L9" s="82"/>
     </row>
@@ -2709,7 +2820,7 @@
   <dimension ref="B1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
@@ -2717,11 +2828,12 @@
     <col min="1" max="1" width="4.5" style="43" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="43" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" style="43" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="43" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="43" customWidth="1"/>
-    <col min="6" max="7" width="13.33203125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="43" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="43" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="43" customWidth="1"/>
+    <col min="7" max="7" width="42.83203125" style="43" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" style="59" customWidth="1"/>
-    <col min="9" max="9" width="33" style="59" customWidth="1"/>
+    <col min="9" max="9" width="46.6640625" style="59" customWidth="1"/>
     <col min="10" max="10" width="103.5" style="43" customWidth="1"/>
     <col min="11" max="16384" width="33.1640625" style="43"/>
   </cols>
@@ -2777,13 +2889,13 @@
         <v>16</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="13" t="s">
         <v>6</v>
@@ -2802,16 +2914,30 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="42"/>
-      <c r="C7" s="99" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="106"/>
+      <c r="C7" s="98" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="117" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="117" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="102">
+        <v>43983</v>
+      </c>
+      <c r="G7" s="117" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="118" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="120" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="42"/>
@@ -2843,7 +2969,7 @@
       <c r="F10" s="48"/>
       <c r="G10" s="48"/>
       <c r="H10" s="48"/>
-      <c r="I10" s="93"/>
+      <c r="I10" s="92"/>
       <c r="J10" s="91"/>
     </row>
     <row r="11" spans="2:10">
@@ -2854,12 +2980,12 @@
       <c r="F11" s="48"/>
       <c r="G11" s="48"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="93"/>
+      <c r="I11" s="92"/>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="42"/>
       <c r="C12" s="48"/>
-      <c r="D12" s="102"/>
+      <c r="D12" s="101"/>
       <c r="E12" s="48"/>
       <c r="F12" s="48"/>
       <c r="G12" s="48"/>
@@ -2886,7 +3012,7 @@
       <c r="F14" s="48"/>
       <c r="G14" s="48"/>
       <c r="H14" s="48"/>
-      <c r="I14" s="93"/>
+      <c r="I14" s="92"/>
       <c r="J14" s="91"/>
     </row>
     <row r="15" spans="2:10">
@@ -2919,13 +3045,13 @@
       <c r="F17" s="48"/>
       <c r="G17" s="48"/>
       <c r="H17" s="48"/>
-      <c r="I17" s="93"/>
+      <c r="I17" s="92"/>
       <c r="J17" s="91"/>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="42"/>
       <c r="C18" s="48"/>
-      <c r="D18" s="102"/>
+      <c r="D18" s="101"/>
       <c r="E18" s="48"/>
       <c r="F18" s="48"/>
       <c r="G18" s="48"/>
@@ -2963,7 +3089,7 @@
       <c r="F21" s="48"/>
       <c r="G21" s="48"/>
       <c r="H21" s="48"/>
-      <c r="I21" s="93"/>
+      <c r="I21" s="92"/>
       <c r="J21" s="91"/>
     </row>
     <row r="22" spans="2:10">
@@ -3007,7 +3133,7 @@
       <c r="F25" s="48"/>
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
-      <c r="I25" s="93"/>
+      <c r="I25" s="92"/>
       <c r="J25" s="91"/>
     </row>
     <row r="26" spans="2:10">
@@ -3020,6 +3146,9 @@
       <c r="C28" s="48"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J7" r:id="rId1" xr:uid="{2028B2DD-E178-EA4E-98D6-B9CA977A0598}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -3029,8 +3158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:M207"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -3092,98 +3221,66 @@
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="76"/>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
+      <c r="C5" s="20" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="6" spans="2:13">
       <c r="B6" s="76"/>
-      <c r="C6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
     </row>
     <row r="7" spans="2:13">
       <c r="B7" s="76"/>
-      <c r="C7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+      <c r="D7" s="119" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="72">
+        <v>12</v>
+      </c>
+      <c r="F7" s="119" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="119" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="76"/>
-      <c r="C8" s="107" t="s">
-        <v>55</v>
-      </c>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="D8" s="119" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="72">
+        <f>E7*3.6</f>
+        <v>43.2</v>
+      </c>
+      <c r="F8" s="119" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="76"/>
-      <c r="C9" s="107" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="71"/>
+      <c r="D9" s="131" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="76"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
+      <c r="D10" s="131" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="76"/>
-      <c r="D11" s="107" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="72">
-        <v>20</v>
-      </c>
-      <c r="F11" s="107" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
+      <c r="E11" s="121"/>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="76"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="76"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="76"/>
-      <c r="C14" s="107"/>
+      <c r="C14" s="105"/>
       <c r="K14" s="71"/>
       <c r="L14" s="71"/>
       <c r="M14" s="71"/>
@@ -3243,7 +3340,7 @@
     <row r="21" spans="2:13" s="20" customFormat="1">
       <c r="B21" s="19"/>
       <c r="C21" s="11" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -3265,8 +3362,8 @@
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="76"/>
-      <c r="C23" s="119" t="s">
-        <v>62</v>
+      <c r="C23" s="132" t="s">
+        <v>81</v>
       </c>
       <c r="D23" s="71"/>
       <c r="E23" s="71"/>
@@ -3281,8 +3378,8 @@
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="76"/>
-      <c r="C24" s="119" t="s">
-        <v>63</v>
+      <c r="C24" s="132" t="s">
+        <v>78</v>
       </c>
       <c r="D24" s="71"/>
       <c r="E24" s="71"/>
@@ -3291,16 +3388,16 @@
       <c r="H24" s="71"/>
       <c r="I24" s="71"/>
       <c r="J24" s="71"/>
-      <c r="K24" s="102"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="102"/>
+      <c r="K24" s="101"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="101"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="76"/>
-      <c r="C25" s="102"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="71"/>
-      <c r="E25" s="102"/>
-      <c r="F25" s="102"/>
+      <c r="E25" s="101"/>
+      <c r="F25" s="101"/>
       <c r="G25" s="71"/>
       <c r="H25" s="71"/>
       <c r="I25" s="71"/>
@@ -3311,25 +3408,27 @@
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="76"/>
-      <c r="C26" s="99"/>
-      <c r="E26" s="120">
-        <v>0.15</v>
-      </c>
-      <c r="F26" s="119" t="s">
-        <v>64</v>
+      <c r="C26" s="98"/>
+      <c r="E26" s="109">
+        <v>0.3</v>
+      </c>
+      <c r="F26" s="132" t="s">
+        <v>75</v>
       </c>
       <c r="K26" s="71"/>
-      <c r="L26" s="71"/>
+      <c r="L26" s="132" t="s">
+        <v>82</v>
+      </c>
       <c r="M26" s="71"/>
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="76"/>
-      <c r="C27" s="99"/>
+      <c r="C27" s="98"/>
       <c r="E27" s="72">
         <v>8760</v>
       </c>
-      <c r="F27" s="119" t="s">
-        <v>65</v>
+      <c r="F27" s="132" t="s">
+        <v>76</v>
       </c>
       <c r="K27" s="71"/>
       <c r="L27" s="71"/>
@@ -3337,12 +3436,12 @@
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="76"/>
-      <c r="E28" s="121">
+      <c r="E28" s="110">
         <f>1-POWER((1-E26),(1/8760))</f>
-        <v>1.8552217117551173E-5</v>
-      </c>
-      <c r="F28" s="118" t="s">
-        <v>66</v>
+        <v>4.0715488903164676E-5</v>
+      </c>
+      <c r="F28" s="131" t="s">
+        <v>77</v>
       </c>
       <c r="K28" s="71"/>
       <c r="L28" s="71"/>
@@ -3369,8 +3468,8 @@
     </row>
     <row r="32" spans="2:13">
       <c r="B32" s="76"/>
-      <c r="C32" s="99"/>
-      <c r="F32" s="99"/>
+      <c r="C32" s="98"/>
+      <c r="F32" s="98"/>
       <c r="K32" s="71"/>
       <c r="L32" s="71"/>
       <c r="M32" s="71"/>
@@ -3383,14 +3482,14 @@
     </row>
     <row r="34" spans="2:13">
       <c r="B34" s="76"/>
-      <c r="C34" s="99"/>
+      <c r="C34" s="98"/>
       <c r="K34" s="71"/>
       <c r="L34" s="71"/>
       <c r="M34" s="71"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="76"/>
-      <c r="F35" s="99"/>
+      <c r="F35" s="98"/>
       <c r="K35" s="71"/>
       <c r="L35" s="71"/>
       <c r="M35" s="71"/>
@@ -3409,40 +3508,64 @@
     </row>
     <row r="38" spans="2:13">
       <c r="B38" s="76"/>
-      <c r="C38" s="99"/>
-      <c r="F38" s="99"/>
+      <c r="C38" s="98"/>
+      <c r="F38" s="98"/>
       <c r="K38" s="71"/>
       <c r="L38" s="71"/>
       <c r="M38" s="71"/>
     </row>
     <row r="39" spans="2:13">
       <c r="B39" s="76"/>
-      <c r="C39" s="99"/>
-      <c r="F39" s="99"/>
+      <c r="C39" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
       <c r="K39" s="71"/>
       <c r="L39" s="71"/>
       <c r="M39" s="71"/>
     </row>
     <row r="40" spans="2:13">
       <c r="B40" s="76"/>
+      <c r="C40" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="71"/>
       <c r="K40" s="71"/>
       <c r="L40" s="71"/>
       <c r="M40" s="71"/>
     </row>
     <row r="41" spans="2:13">
       <c r="B41" s="76"/>
+      <c r="C41" s="98"/>
+      <c r="F41" s="98"/>
       <c r="K41" s="71"/>
       <c r="L41" s="71"/>
       <c r="M41" s="71"/>
     </row>
     <row r="42" spans="2:13">
       <c r="B42" s="76"/>
+      <c r="C42" s="131" t="s">
+        <v>80</v>
+      </c>
       <c r="K42" s="71"/>
       <c r="L42" s="71"/>
       <c r="M42" s="71"/>
     </row>
     <row r="43" spans="2:13">
       <c r="B43" s="76"/>
+      <c r="C43" s="105"/>
       <c r="K43" s="71"/>
       <c r="L43" s="71"/>
       <c r="M43" s="71"/>
@@ -3455,6 +3578,15 @@
     </row>
     <row r="45" spans="2:13">
       <c r="B45" s="76"/>
+      <c r="D45" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="72">
+        <v>20</v>
+      </c>
+      <c r="F45" s="105" t="s">
+        <v>14</v>
+      </c>
       <c r="K45" s="71"/>
       <c r="L45" s="71"/>
       <c r="M45" s="71"/>
@@ -3467,14 +3599,6 @@
     </row>
     <row r="47" spans="2:13">
       <c r="B47" s="76"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="71"/>
       <c r="K47" s="71"/>
       <c r="L47" s="71"/>
       <c r="M47" s="71"/>
@@ -3639,11 +3763,11 @@
     </row>
     <row r="65" spans="2:13">
       <c r="B65" s="76"/>
-      <c r="C65" s="97"/>
+      <c r="C65" s="96"/>
       <c r="D65" s="71"/>
-      <c r="E65" s="97"/>
+      <c r="E65" s="96"/>
       <c r="F65" s="71"/>
-      <c r="G65" s="97"/>
+      <c r="G65" s="96"/>
       <c r="H65" s="71"/>
       <c r="I65" s="71"/>
       <c r="J65" s="71"/>
@@ -3653,11 +3777,11 @@
     </row>
     <row r="66" spans="2:13">
       <c r="B66" s="76"/>
-      <c r="C66" s="97"/>
+      <c r="C66" s="96"/>
       <c r="D66" s="71"/>
       <c r="E66" s="71"/>
       <c r="F66" s="71"/>
-      <c r="G66" s="97"/>
+      <c r="G66" s="96"/>
       <c r="H66" s="71"/>
       <c r="I66" s="71"/>
       <c r="J66" s="71"/>
@@ -3671,7 +3795,7 @@
       <c r="D67" s="71"/>
       <c r="E67" s="71"/>
       <c r="F67" s="71"/>
-      <c r="G67" s="97"/>
+      <c r="G67" s="96"/>
       <c r="H67" s="71"/>
       <c r="I67" s="71"/>
       <c r="J67" s="71"/>
@@ -3695,11 +3819,11 @@
     </row>
     <row r="69" spans="2:13">
       <c r="B69" s="76"/>
-      <c r="C69" s="97"/>
+      <c r="C69" s="96"/>
       <c r="D69" s="71"/>
       <c r="E69" s="71"/>
       <c r="F69" s="71"/>
-      <c r="G69" s="98"/>
+      <c r="G69" s="97"/>
       <c r="H69" s="71"/>
       <c r="I69" s="71"/>
       <c r="J69" s="71"/>
@@ -3723,12 +3847,12 @@
     </row>
     <row r="71" spans="2:13">
       <c r="B71" s="76"/>
-      <c r="C71" s="97"/>
+      <c r="C71" s="96"/>
       <c r="D71" s="71"/>
       <c r="E71" s="71"/>
       <c r="F71" s="71"/>
-      <c r="G71" s="97"/>
-      <c r="H71" s="97"/>
+      <c r="G71" s="96"/>
+      <c r="H71" s="96"/>
       <c r="I71" s="71"/>
       <c r="J71" s="71"/>
       <c r="K71" s="71"/>
@@ -3749,7 +3873,7 @@
     </row>
     <row r="73" spans="2:13">
       <c r="B73" s="76"/>
-      <c r="C73" s="97"/>
+      <c r="C73" s="96"/>
       <c r="F73" s="71"/>
       <c r="G73" s="71"/>
       <c r="H73" s="71"/>

</xml_diff>